<commit_message>
[MS-OXWSFOLD] Add new capture codes and update capture codes
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites\ExchangeWebServices\Docs\MS-OXWSFOLD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EWS\MS-OXWSFOLD\AddAdapterAndTestCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -10057,7 +10057,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M1046"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B324" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E334" sqref="E334"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -13511,7 +13513,7 @@
       <c r="I142" s="27"/>
     </row>
     <row r="143" spans="1:9" ht="105">
-      <c r="A143" s="25" t="s">
+      <c r="A143" s="18" t="s">
         <v>222</v>
       </c>
       <c r="B143" s="20" t="s">
@@ -13538,7 +13540,7 @@
       </c>
     </row>
     <row r="144" spans="1:9" ht="30">
-      <c r="A144" s="25" t="s">
+      <c r="A144" s="18" t="s">
         <v>223</v>
       </c>
       <c r="B144" s="26" t="s">
@@ -13559,13 +13561,13 @@
       <c r="G144" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H144" s="25" t="s">
-        <v>20</v>
+      <c r="H144" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I144" s="27"/>
     </row>
     <row r="145" spans="1:9" ht="30">
-      <c r="A145" s="25" t="s">
+      <c r="A145" s="18" t="s">
         <v>224</v>
       </c>
       <c r="B145" s="26" t="s">
@@ -13586,8 +13588,8 @@
       <c r="G145" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H145" s="25" t="s">
-        <v>20</v>
+      <c r="H145" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I145" s="27"/>
     </row>
@@ -13613,8 +13615,8 @@
       <c r="G146" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H146" s="25" t="s">
-        <v>20</v>
+      <c r="H146" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I146" s="27"/>
     </row>
@@ -13640,8 +13642,8 @@
       <c r="G147" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H147" s="25" t="s">
-        <v>20</v>
+      <c r="H147" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I147" s="27"/>
     </row>
@@ -13667,13 +13669,13 @@
       <c r="G148" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H148" s="25" t="s">
-        <v>20</v>
+      <c r="H148" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I148" s="27"/>
     </row>
     <row r="149" spans="1:9" ht="30">
-      <c r="A149" s="25" t="s">
+      <c r="A149" s="18" t="s">
         <v>228</v>
       </c>
       <c r="B149" s="26" t="s">
@@ -13694,8 +13696,8 @@
       <c r="G149" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H149" s="25" t="s">
-        <v>20</v>
+      <c r="H149" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I149" s="27"/>
     </row>
@@ -14070,7 +14072,7 @@
       </c>
     </row>
     <row r="164" spans="1:9">
-      <c r="A164" s="25" t="s">
+      <c r="A164" s="18" t="s">
         <v>242</v>
       </c>
       <c r="B164" s="26" t="s">
@@ -14089,8 +14091,8 @@
       <c r="G164" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H164" s="25" t="s">
-        <v>20</v>
+      <c r="H164" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I164" s="27"/>
     </row>
@@ -14141,8 +14143,8 @@
       <c r="G166" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H166" s="25" t="s">
-        <v>20</v>
+      <c r="H166" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I166" s="27"/>
     </row>
@@ -14194,7 +14196,7 @@
         <v>15</v>
       </c>
       <c r="H168" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I168" s="16"/>
     </row>
@@ -17503,8 +17505,8 @@
       <c r="G298" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H298" s="25" t="s">
-        <v>20</v>
+      <c r="H298" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I298" s="27"/>
     </row>
@@ -17530,13 +17532,13 @@
       <c r="G299" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H299" s="25" t="s">
-        <v>20</v>
+      <c r="H299" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I299" s="27"/>
     </row>
     <row r="300" spans="1:9" ht="30">
-      <c r="A300" s="25" t="s">
+      <c r="A300" s="18" t="s">
         <v>297</v>
       </c>
       <c r="B300" s="26" t="s">
@@ -17557,8 +17559,8 @@
       <c r="G300" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H300" s="25" t="s">
-        <v>20</v>
+      <c r="H300" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I300" s="27"/>
     </row>
@@ -17842,7 +17844,7 @@
       <c r="I311" s="27"/>
     </row>
     <row r="312" spans="1:9" ht="30">
-      <c r="A312" s="25" t="s">
+      <c r="A312" s="18" t="s">
         <v>309</v>
       </c>
       <c r="B312" s="26" t="s">
@@ -18325,7 +18327,7 @@
       <c r="I330" s="27"/>
     </row>
     <row r="331" spans="1:9" ht="30">
-      <c r="A331" s="25" t="s">
+      <c r="A331" s="18" t="s">
         <v>328</v>
       </c>
       <c r="B331" s="26" t="s">
@@ -18344,8 +18346,8 @@
       <c r="G331" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H331" s="25" t="s">
-        <v>20</v>
+      <c r="H331" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I331" s="27"/>
     </row>
@@ -18400,7 +18402,7 @@
       <c r="I333" s="27"/>
     </row>
     <row r="334" spans="1:9" ht="30">
-      <c r="A334" s="25" t="s">
+      <c r="A334" s="18" t="s">
         <v>331</v>
       </c>
       <c r="B334" s="26" t="s">
@@ -18419,8 +18421,8 @@
       <c r="G334" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H334" s="25" t="s">
-        <v>20</v>
+      <c r="H334" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I334" s="27"/>
     </row>
@@ -36602,6 +36604,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -36650,15 +36661,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
@@ -36674,6 +36676,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36686,12 +36696,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-OXWSFOLD]: Update RS that blocked by TDQ
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EWS\MS-OXWSFOLD\AddAdapterAndTestCase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites\ExchangeWebServices\Docs\MS-OXWSFOLD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -10057,9 +10057,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M1046"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B324" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E334" sqref="E334"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -11988,7 +11986,7 @@
         <v>15</v>
       </c>
       <c r="H82" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I82" s="27"/>
     </row>
@@ -12038,7 +12036,7 @@
         <v>15</v>
       </c>
       <c r="H84" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I84" s="27"/>
     </row>
@@ -18397,7 +18395,7 @@
         <v>15</v>
       </c>
       <c r="H333" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I333" s="27"/>
     </row>
@@ -18597,7 +18595,7 @@
         <v>15</v>
       </c>
       <c r="H341" s="25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I341" s="27"/>
     </row>
@@ -36604,15 +36602,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -36661,6 +36650,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
@@ -36676,14 +36674,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36696,4 +36686,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-OXWSFOLD: Update RS, adapter and test cases.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EWS\MS-OXWSFOLD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EWS\MS-OXWSFOLD\AddAdapterAndTestCase\0321\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -8559,13 +8559,13 @@
     <t>MS-OXWSFOLD_R11521:i</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] [CanRenameOrMove]A value of "true" indicates that the managed folder can be renamed [or moved]. (Exchange Server 2013 and above follow this behavior.)</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] [CanRenameOrMove]A value of "true" indicates that the managed folder can be [renamed or] moved. (Exchange Server 2013 and above follow this behavior.)</t>
-  </si>
-  <si>
     <t>[In Appendix C: Product Behavior] Implementation does use StorageQuota which is the storage quota for a managed folder. (Exchange Server 2010 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support value of "true" for CanRenameOrMove to indicate that the managed folder can be renamed. (Exchange 2013 and above follow this behavior.)</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support value of "true" for CanRenameOrMove to indicate that the managed folder can be moved. (Exchange 2013 and above follow this behavior.)</t>
   </si>
 </sst>
 </file>
@@ -9006,288 +9006,6 @@
   <dxfs count="71">
     <dxf>
       <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -9605,6 +9323,288 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -9734,34 +9734,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1049" tableType="xml" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1049" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
   <autoFilter ref="A19:I1049"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="68">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="67">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="66">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="65">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="64">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="63">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="62">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="61">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="60">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -9770,12 +9770,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="56"/>
-    <tableColumn id="2" name="Test" dataDxfId="55"/>
-    <tableColumn id="3" name="Description" dataDxfId="54"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10105,9 +10105,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M1051"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D309" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H316" sqref="H316"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -34637,7 +34635,7 @@
         <v>1137</v>
       </c>
       <c r="C978" s="16" t="s">
-        <v>2340</v>
+        <v>2341</v>
       </c>
       <c r="D978" s="18" t="s">
         <v>2338</v>
@@ -34666,7 +34664,7 @@
         <v>1137</v>
       </c>
       <c r="C979" s="16" t="s">
-        <v>2341</v>
+        <v>2342</v>
       </c>
       <c r="D979" s="18" t="s">
         <v>2339</v>
@@ -34695,7 +34693,7 @@
         <v>1137</v>
       </c>
       <c r="C980" s="16" t="s">
-        <v>2342</v>
+        <v>2340</v>
       </c>
       <c r="D980" s="18" t="s">
         <v>2327</v>
@@ -36557,202 +36555,202 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1004:B1004 A20:H45 D1004:I1004 A1005:I1034 I1003:I1028 A1036:I1044 A1046:I1049 A34:I1003">
-    <cfRule type="expression" dxfId="53" priority="93">
+    <cfRule type="expression" dxfId="70" priority="93">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="94">
+    <cfRule type="expression" dxfId="69" priority="94">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="101">
+    <cfRule type="expression" dxfId="68" priority="101">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1004:B1004 A20:H45 D1004:I1004 A1005:I1034 I1003:I1028 A1036:I1044 A1046:I1049 A34:I1003">
-    <cfRule type="expression" dxfId="50" priority="47">
+    <cfRule type="expression" dxfId="67" priority="47">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="48">
+    <cfRule type="expression" dxfId="66" priority="48">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="49">
+    <cfRule type="expression" dxfId="65" priority="49">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1036:F1044 F1046:F1049 F20:F1034">
-    <cfRule type="expression" dxfId="47" priority="53">
+    <cfRule type="expression" dxfId="64" priority="53">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="54">
+    <cfRule type="expression" dxfId="63" priority="54">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I45">
-    <cfRule type="expression" dxfId="45" priority="44">
+    <cfRule type="expression" dxfId="62" priority="44">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="45">
+    <cfRule type="expression" dxfId="61" priority="45">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="46">
+    <cfRule type="expression" dxfId="60" priority="46">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I45">
-    <cfRule type="expression" dxfId="42" priority="41">
+    <cfRule type="expression" dxfId="59" priority="41">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="42">
+    <cfRule type="expression" dxfId="58" priority="42">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="43">
+    <cfRule type="expression" dxfId="57" priority="43">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1004">
-    <cfRule type="expression" dxfId="39" priority="38">
+    <cfRule type="expression" dxfId="56" priority="38">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="55" priority="39">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="40">
+    <cfRule type="expression" dxfId="54" priority="40">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1004">
-    <cfRule type="expression" dxfId="36" priority="35">
+    <cfRule type="expression" dxfId="53" priority="35">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="52" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="37">
+    <cfRule type="expression" dxfId="51" priority="37">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1035:I1035">
-    <cfRule type="expression" dxfId="33" priority="32">
+    <cfRule type="expression" dxfId="50" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="33">
+    <cfRule type="expression" dxfId="49" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="34">
+    <cfRule type="expression" dxfId="48" priority="34">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1035:I1035">
-    <cfRule type="expression" dxfId="30" priority="27">
+    <cfRule type="expression" dxfId="47" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="28">
+    <cfRule type="expression" dxfId="46" priority="28">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="45" priority="29">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1035">
-    <cfRule type="expression" dxfId="27" priority="30">
+    <cfRule type="expression" dxfId="44" priority="30">
       <formula>NOT(VLOOKUP(F1035,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="31">
+    <cfRule type="expression" dxfId="43" priority="31">
       <formula>(VLOOKUP(F1035,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1035:C1035">
-    <cfRule type="expression" dxfId="25" priority="21">
+    <cfRule type="expression" dxfId="42" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="22">
+    <cfRule type="expression" dxfId="41" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="23">
+    <cfRule type="expression" dxfId="40" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1035:C1035">
-    <cfRule type="expression" dxfId="22" priority="24">
+    <cfRule type="expression" dxfId="39" priority="24">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="25">
+    <cfRule type="expression" dxfId="38" priority="25">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="26">
+    <cfRule type="expression" dxfId="37" priority="26">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1045:I1045">
-    <cfRule type="expression" dxfId="19" priority="18">
+    <cfRule type="expression" dxfId="36" priority="18">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="35" priority="19">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="20">
+    <cfRule type="expression" dxfId="34" priority="20">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1045:I1045">
-    <cfRule type="expression" dxfId="16" priority="13">
+    <cfRule type="expression" dxfId="33" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="14">
+    <cfRule type="expression" dxfId="32" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1045">
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="30" priority="16">
       <formula>NOT(VLOOKUP(F1045,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="17">
+    <cfRule type="expression" dxfId="29" priority="17">
       <formula>(VLOOKUP(F1045,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1045">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="28" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="26" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1045:D1045">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="25" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11">
+    <cfRule type="expression" dxfId="24" priority="11">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12">
+    <cfRule type="expression" dxfId="23" priority="12">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1045:D1045">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="22" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="21" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="20" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1045">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="18" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="17" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36793,12 +36791,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36851,15 +36846,24 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -36880,15 +36884,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix watchman issues for MS-OXWSFOLD.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
@@ -8515,12 +8515,6 @@
     <t>MS-OXWSFOLD_R10521:i</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support value of "false" for CanRenameOrMove to indicate that the managed folder can not be moved. (Exchange 2013 and above follow this behavior.)</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support value of "false" for CanRenameOrMove to indicate that the managed folder can not be renamed. (Exchange 2013 and above follow this behavior.)</t>
-  </si>
-  <si>
     <t>MS-OXWSFOLD_R10511:i</t>
   </si>
   <si>
@@ -8579,6 +8573,12 @@
   </si>
   <si>
     <t>MS-OXWSCDATA_R83</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support value of "false" for CanRenameOrMove to indicate that the managed folder can not be renamed. (Exchange 2007, Exchange 2010 and Exchange2013 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support value of "false" for CanRenameOrMove to indicate that the managed folder can not be moved. (Exchange 2007, Exchange 2010 and Exchange2013 follow this behavior)</t>
   </si>
 </sst>
 </file>
@@ -10582,7 +10582,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="54" t="s">
-        <v>2343</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="19" customFormat="1" ht="60">
@@ -13829,7 +13829,7 @@
         <v>17</v>
       </c>
       <c r="I143" s="16" t="s">
-        <v>2333</v>
+        <v>2331</v>
       </c>
       <c r="J143" s="53"/>
     </row>
@@ -18083,7 +18083,7 @@
         <v>17</v>
       </c>
       <c r="I303" s="16" t="s">
-        <v>2341</v>
+        <v>2339</v>
       </c>
       <c r="J303" s="53"/>
     </row>
@@ -18170,7 +18170,7 @@
         <v>15</v>
       </c>
       <c r="H306" s="18" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I306" s="16" t="s">
         <v>2323</v>
@@ -18200,10 +18200,10 @@
         <v>15</v>
       </c>
       <c r="H307" s="18" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I307" s="16" t="s">
-        <v>2332</v>
+        <v>2330</v>
       </c>
       <c r="J307" s="53"/>
     </row>
@@ -27731,7 +27731,7 @@
         <v>17</v>
       </c>
       <c r="I672" s="16" t="s">
-        <v>2334</v>
+        <v>2332</v>
       </c>
       <c r="J672" s="53"/>
     </row>
@@ -29197,7 +29197,7 @@
         <v>17</v>
       </c>
       <c r="I728" s="16" t="s">
-        <v>2335</v>
+        <v>2333</v>
       </c>
       <c r="J728" s="53"/>
     </row>
@@ -30977,7 +30977,7 @@
         <v>17</v>
       </c>
       <c r="I796" s="16" t="s">
-        <v>2336</v>
+        <v>2334</v>
       </c>
       <c r="J796" s="53"/>
     </row>
@@ -35767,16 +35767,16 @@
     </row>
     <row r="980" spans="1:10" ht="45">
       <c r="A980" s="18" t="s">
-        <v>2330</v>
+        <v>2328</v>
       </c>
       <c r="B980" s="26" t="s">
         <v>1135</v>
       </c>
       <c r="C980" s="16" t="s">
-        <v>2327</v>
+        <v>2346</v>
       </c>
       <c r="D980" s="18" t="s">
-        <v>2328</v>
+        <v>2326</v>
       </c>
       <c r="E980" s="25" t="s">
         <v>22</v>
@@ -35797,16 +35797,16 @@
     </row>
     <row r="981" spans="1:10" ht="45">
       <c r="A981" s="18" t="s">
-        <v>2331</v>
+        <v>2329</v>
       </c>
       <c r="B981" s="26" t="s">
         <v>1135</v>
       </c>
       <c r="C981" s="16" t="s">
-        <v>2326</v>
+        <v>2347</v>
       </c>
       <c r="D981" s="18" t="s">
-        <v>2329</v>
+        <v>2327</v>
       </c>
       <c r="E981" s="25" t="s">
         <v>22</v>
@@ -36739,7 +36739,7 @@
         <v>17</v>
       </c>
       <c r="I1014" s="16" t="s">
-        <v>2337</v>
+        <v>2335</v>
       </c>
       <c r="J1014" s="53"/>
     </row>
@@ -37137,7 +37137,7 @@
         <v>17</v>
       </c>
       <c r="I1029" s="16" t="s">
-        <v>2338</v>
+        <v>2336</v>
       </c>
       <c r="J1029" s="53"/>
     </row>
@@ -37165,7 +37165,7 @@
         <v>17</v>
       </c>
       <c r="I1030" s="16" t="s">
-        <v>2339</v>
+        <v>2337</v>
       </c>
       <c r="J1030" s="53"/>
     </row>
@@ -37277,13 +37277,13 @@
         <v>17</v>
       </c>
       <c r="I1034" s="16" t="s">
-        <v>2340</v>
+        <v>2338</v>
       </c>
       <c r="J1034" s="53"/>
     </row>
     <row r="1035" spans="1:10" ht="45">
       <c r="A1035" s="46" t="s">
-        <v>2346</v>
+        <v>2344</v>
       </c>
       <c r="B1035" s="47" t="s">
         <v>1137</v>
@@ -37305,13 +37305,13 @@
         <v>17</v>
       </c>
       <c r="I1035" s="16" t="s">
-        <v>2345</v>
+        <v>2343</v>
       </c>
       <c r="J1035" s="53"/>
     </row>
     <row r="1036" spans="1:10" ht="409.5">
       <c r="A1036" s="18" t="s">
-        <v>2347</v>
+        <v>2345</v>
       </c>
       <c r="B1036" s="20" t="s">
         <v>1137</v>
@@ -37581,13 +37581,13 @@
     </row>
     <row r="1046" spans="1:10" ht="45">
       <c r="A1046" s="51" t="s">
-        <v>2342</v>
+        <v>2340</v>
       </c>
       <c r="B1046" s="50" t="s">
         <v>1135</v>
       </c>
       <c r="C1046" s="52" t="s">
-        <v>2344</v>
+        <v>2342</v>
       </c>
       <c r="D1046" s="49" t="s">
         <v>2300</v>
@@ -38025,21 +38025,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -38088,10 +38073,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -38111,16 +38118,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix watchman issues for MS-OXWSCORE and MS-OXWSFOLD.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
@@ -8542,9 +8542,6 @@
     <t>Verified by derived requirements: MS-OXWSFOLD_R42101, MS-OXWSFOLD_R42102, MS-OXWSFOLD_R42103, MS-OXWSFOLD_R42104, MS-OXWSFOLD_R42105.</t>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-OXWSFOLD_R8101011, MS-OXWSFOLD_R8101012.</t>
-  </si>
-  <si>
     <t>Verified by derived requirement: MS-OXWSFOLD_R42101.</t>
   </si>
   <si>
@@ -8579,6 +8576,9 @@
   </si>
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does support value of "false" for CanRenameOrMove to indicate that the managed folder can not be moved. (Exchange 2007, Exchange 2010 and Exchange2013 follow this behavior)</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXWSFOLD_R8101011, MS-OXWSFOLD_R8101012.</t>
   </si>
 </sst>
 </file>
@@ -10227,7 +10227,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M1052"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -10582,7 +10584,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="54" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="19" customFormat="1" ht="60">
@@ -14350,7 +14352,7 @@
         <v>15</v>
       </c>
       <c r="H162" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I162" s="16"/>
       <c r="J162" s="53"/>
@@ -14376,7 +14378,7 @@
         <v>15</v>
       </c>
       <c r="H163" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I163" s="16"/>
       <c r="J163" s="53"/>
@@ -14428,7 +14430,7 @@
         <v>15</v>
       </c>
       <c r="H165" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I165" s="16"/>
       <c r="J165" s="53"/>
@@ -14480,7 +14482,7 @@
         <v>15</v>
       </c>
       <c r="H167" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I167" s="16"/>
       <c r="J167" s="53"/>
@@ -18083,7 +18085,7 @@
         <v>17</v>
       </c>
       <c r="I303" s="16" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="J303" s="53"/>
     </row>
@@ -18170,7 +18172,7 @@
         <v>15</v>
       </c>
       <c r="H306" s="18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I306" s="16" t="s">
         <v>2323</v>
@@ -18200,7 +18202,7 @@
         <v>15</v>
       </c>
       <c r="H307" s="18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I307" s="16" t="s">
         <v>2330</v>
@@ -19206,7 +19208,7 @@
       <c r="J345" s="53"/>
     </row>
     <row r="346" spans="1:10">
-      <c r="A346" s="25" t="s">
+      <c r="A346" s="18" t="s">
         <v>341</v>
       </c>
       <c r="B346" s="26" t="s">
@@ -19225,8 +19227,8 @@
       <c r="G346" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H346" s="25" t="s">
-        <v>18</v>
+      <c r="H346" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="I346" s="27"/>
       <c r="J346" s="53"/>
@@ -20686,7 +20688,7 @@
       <c r="J401" s="53"/>
     </row>
     <row r="402" spans="1:10" ht="30">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="18" t="s">
         <v>401</v>
       </c>
       <c r="B402" s="26" t="s">
@@ -26642,7 +26644,7 @@
       <c r="J630" s="53"/>
     </row>
     <row r="631" spans="1:10" ht="45">
-      <c r="A631" s="25" t="s">
+      <c r="A631" s="18" t="s">
         <v>622</v>
       </c>
       <c r="B631" s="26" t="s">
@@ -27840,7 +27842,7 @@
         <v>15</v>
       </c>
       <c r="H676" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I676" s="16"/>
       <c r="J676" s="53"/>
@@ -35773,7 +35775,7 @@
         <v>1135</v>
       </c>
       <c r="C980" s="16" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="D980" s="18" t="s">
         <v>2326</v>
@@ -35803,7 +35805,7 @@
         <v>1135</v>
       </c>
       <c r="C981" s="16" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="D981" s="18" t="s">
         <v>2327</v>
@@ -36342,7 +36344,7 @@
       <c r="J999" s="53"/>
     </row>
     <row r="1000" spans="1:10" ht="45">
-      <c r="A1000" s="25" t="s">
+      <c r="A1000" s="18" t="s">
         <v>970</v>
       </c>
       <c r="B1000" s="26" t="s">
@@ -36739,7 +36741,7 @@
         <v>17</v>
       </c>
       <c r="I1014" s="16" t="s">
-        <v>2335</v>
+        <v>2347</v>
       </c>
       <c r="J1014" s="53"/>
     </row>
@@ -37137,7 +37139,7 @@
         <v>17</v>
       </c>
       <c r="I1029" s="16" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="J1029" s="53"/>
     </row>
@@ -37165,7 +37167,7 @@
         <v>17</v>
       </c>
       <c r="I1030" s="16" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="J1030" s="53"/>
     </row>
@@ -37277,13 +37279,13 @@
         <v>17</v>
       </c>
       <c r="I1034" s="16" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="J1034" s="53"/>
     </row>
     <row r="1035" spans="1:10" ht="45">
       <c r="A1035" s="46" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="B1035" s="47" t="s">
         <v>1137</v>
@@ -37305,13 +37307,13 @@
         <v>17</v>
       </c>
       <c r="I1035" s="16" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="J1035" s="53"/>
     </row>
     <row r="1036" spans="1:10" ht="409.5">
       <c r="A1036" s="18" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="B1036" s="20" t="s">
         <v>1137</v>
@@ -37336,7 +37338,7 @@
       <c r="J1036" s="53"/>
     </row>
     <row r="1037" spans="1:10" ht="45">
-      <c r="A1037" s="25" t="s">
+      <c r="A1037" s="18" t="s">
         <v>978</v>
       </c>
       <c r="B1037" s="20" t="s">
@@ -37355,8 +37357,8 @@
       <c r="G1037" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H1037" s="25" t="s">
-        <v>20</v>
+      <c r="H1037" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="I1037" s="27"/>
       <c r="J1037" s="53"/>
@@ -37581,13 +37583,13 @@
     </row>
     <row r="1046" spans="1:10" ht="45">
       <c r="A1046" s="51" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="B1046" s="50" t="s">
         <v>1135</v>
       </c>
       <c r="C1046" s="52" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="D1046" s="49" t="s">
         <v>2300</v>
@@ -38025,6 +38027,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -38073,32 +38090,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -38118,9 +38113,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix watchman issue for MS-OXWSCORE and MS-OXWSFOLD
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSFOLD/MS-OXWSFOLD_RequirementSpecification.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7426" uniqueCount="2348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7425" uniqueCount="2347">
   <si>
     <t>Req ID</t>
   </si>
@@ -8549,9 +8549,6 @@
   </si>
   <si>
     <t>Verified by derived requirements: MS-OXWSFOLD_R34303, MS-OXWSFOLD_R37803.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirements: MS-OXWSFOLD_R1052, MS-OXWSFOLD_R10521, MS-OXWSFOLD_R10511, MS-OXWSFOLD_R105111.</t>
   </si>
   <si>
     <t>MS-OXWSCDATA_R4000</t>
@@ -10227,9 +10224,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M1052"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -10584,7 +10579,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="54" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="19" customFormat="1" ht="60">
@@ -18061,7 +18056,7 @@
       <c r="I302" s="27"/>
       <c r="J302" s="53"/>
     </row>
-    <row r="303" spans="1:10" ht="90">
+    <row r="303" spans="1:10" ht="30">
       <c r="A303" s="18" t="s">
         <v>300</v>
       </c>
@@ -18084,9 +18079,7 @@
       <c r="H303" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I303" s="16" t="s">
-        <v>2338</v>
-      </c>
+      <c r="I303" s="16"/>
       <c r="J303" s="53"/>
     </row>
     <row r="304" spans="1:10" ht="45">
@@ -35775,7 +35768,7 @@
         <v>1135</v>
       </c>
       <c r="C980" s="16" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="D980" s="18" t="s">
         <v>2326</v>
@@ -35805,7 +35798,7 @@
         <v>1135</v>
       </c>
       <c r="C981" s="16" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="D981" s="18" t="s">
         <v>2327</v>
@@ -36741,7 +36734,7 @@
         <v>17</v>
       </c>
       <c r="I1014" s="16" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="J1014" s="53"/>
     </row>
@@ -37285,7 +37278,7 @@
     </row>
     <row r="1035" spans="1:10" ht="45">
       <c r="A1035" s="46" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="B1035" s="47" t="s">
         <v>1137</v>
@@ -37307,13 +37300,13 @@
         <v>17</v>
       </c>
       <c r="I1035" s="16" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="J1035" s="53"/>
     </row>
     <row r="1036" spans="1:10" ht="409.5">
       <c r="A1036" s="18" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="B1036" s="20" t="s">
         <v>1137</v>
@@ -37583,13 +37576,13 @@
     </row>
     <row r="1046" spans="1:10" ht="45">
       <c r="A1046" s="51" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="B1046" s="50" t="s">
         <v>1135</v>
       </c>
       <c r="C1046" s="52" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="D1046" s="49" t="s">
         <v>2300</v>
@@ -38027,21 +38020,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -38090,10 +38068,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -38113,16 +38113,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>